<commit_message>
bulk upload sample file changes
</commit_message>
<xml_diff>
--- a/MDO/client-assets/assets/common/user-approvals-upload-sample/user-approvals-upload-sample.xlsx
+++ b/MDO/client-assets/assets/common/user-approvals-upload-sample/user-approvals-upload-sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IGOT_NIC\Assets\forked\sunbird-cb-portal-assets\MDO\client-assets\assets\common\user-approvals-upload-sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KB-iGot\Fork Repo\sunbird-cb-portal-assets\MDO\client-assets\assets\common\user-approvals-upload-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFD6ECB-09C4-41C2-8F39-DB27A659F1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D26B17-713E-4B8B-8061-002F21C3216C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,10 +99,10 @@
     <t>sahil11@yopmail.com</t>
   </si>
   <si>
-    <t>Rozgar Mela, Finance</t>
-  </si>
-  <si>
     <t>eHRMSN</t>
+  </si>
+  <si>
+    <t>Rozgar Mela; Finance</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -644,10 +646,10 @@
         <v>12</v>
       </c>
       <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
         <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>